<commit_message>
bug fixed in editing, was not saved
</commit_message>
<xml_diff>
--- a/files/system/import-task-libraries-sample.xlsx
+++ b/files/system/import-task-libraries-sample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t>Docking and undocking</t>
-  </si>
-  <si>
-    <t>General</t>
   </si>
   <si>
     <t>G01</t>
@@ -232,6 +229,9 @@
 •	Pilots
 •	Tugs</t>
     </r>
+  </si>
+  <si>
+    <t>General &amp; Docking</t>
   </si>
 </sst>
 </file>
@@ -584,8 +584,8 @@
   <dimension ref="A1:AH66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:AH66"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,16 +726,16 @@
         <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="8"/>
@@ -744,7 +744,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>33</v>
@@ -797,22 +797,22 @@
     </row>
     <row r="3" spans="1:34" ht="195" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>32</v>
@@ -866,24 +866,24 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>32</v>
@@ -936,17 +936,17 @@
     </row>
     <row r="5" spans="1:34" ht="300" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -955,7 +955,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
bug fixed in importing xlsx in task library, sample updated
</commit_message>
<xml_diff>
--- a/files/system/import-task-libraries-sample.xlsx
+++ b/files/system/import-task-libraries-sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\xampp\htdocs\peerfleet\files\system\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\xampp\htdocs\Peerfleet-git\files\system\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t>Risk assessment</t>
-  </si>
-  <si>
-    <t>Maker</t>
   </si>
   <si>
     <t>Type</t>
@@ -232,6 +229,9 @@
   </si>
   <si>
     <t>General &amp; Docking</t>
+  </si>
+  <si>
+    <t>Marker</t>
   </si>
 </sst>
 </file>
@@ -583,9 +583,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,7 +646,7 @@
         <v>14</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>13</v>
@@ -700,42 +700,42 @@
         <v>27</v>
       </c>
       <c r="AB1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC1" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="AC1" s="7" t="s">
-        <v>35</v>
       </c>
       <c r="AD1" s="7" t="s">
         <v>28</v>
       </c>
       <c r="AE1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="AH1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:34" ht="345" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="8"/>
@@ -744,10 +744,10 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
@@ -797,25 +797,25 @@
     </row>
     <row r="3" spans="1:34" ht="195" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
@@ -866,27 +866,27 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
@@ -936,17 +936,17 @@
     </row>
     <row r="5" spans="1:34" ht="300" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -955,10 +955,10 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N5" s="3" t="s">
         <v>6</v>

</xml_diff>